<commit_message>
reparando errores de conexion
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cacuna\Desktop\Hallazgos Pos-Despliegue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D4B162-EF14-4672-966F-1792AFDF892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2186B01F-2336-42A4-9A4E-087533FFCE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Cambio en las variables de Pais</t>
   </si>
   <si>
-    <t>El ReferenceID cambia a de 167 a 144</t>
-  </si>
-  <si>
     <t>Error Codigo Fuente</t>
   </si>
   <si>
@@ -169,6 +166,21 @@
   </si>
   <si>
     <t>Abierta</t>
+  </si>
+  <si>
+    <t>Bloqueo de cuenta innactivo</t>
+  </si>
+  <si>
+    <t>Contador de numero de intentos permitidos</t>
+  </si>
+  <si>
+    <t>El ReferenceID cambia a de 167 a 141</t>
+  </si>
+  <si>
+    <t>El usuario deberá vizualizar la cantidad intentos permitidos asi mismo redirigirlo a una pagina donde le notifique que la cuenta fue bloqueda.</t>
+  </si>
+  <si>
+    <t>Error de codigo fuente</t>
   </si>
 </sst>
 </file>
@@ -247,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,6 +290,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -631,7 +646,7 @@
         <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -652,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -673,7 +688,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -694,7 +709,7 @@
         <v>37</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -715,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -736,7 +751,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -757,7 +772,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -778,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -799,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -820,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -828,20 +843,41 @@
       <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="G11" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="9" t="s">
         <v>44</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quitando los campos departamentos innecesarios
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BAFD23-9873-45DF-868A-5471982F9EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C80E115-09E3-4E24-993A-64534CBD34FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modificacion pre-resolucion" sheetId="3" r:id="rId1"/>
+    <sheet name="hallazgos" sheetId="1" r:id="rId2"/>
+    <sheet name="RF" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="106">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -250,13 +252,115 @@
   </si>
   <si>
     <t>Integracion incompleta</t>
+  </si>
+  <si>
+    <t>50/100</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>RF2: Agregar de Campos adicionales a la BD, (Cotiza en Bolsa), Dignatarios/DIRECTORES/ Apoderados</t>
+  </si>
+  <si>
+    <t>RF3: verificacion de en lista ofac/onu cliente_nat/rz/apoderado/rep/bf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF4: Generar constancia de barrido  individuales </t>
+  </si>
+  <si>
+    <t>RF5: Generar reportes de constancia de barridos mensuales (# cliente / hora de barrido / fecha)</t>
+  </si>
+  <si>
+    <t>RF6: Integrar a constancia indivuales, (RZ, Cliente_nat, RL, AC, BF, Empleados, Proveedores)</t>
+  </si>
+  <si>
+    <t>RF7: Integrar la fecha proxima a vencerse de los Representante Legales</t>
+  </si>
+  <si>
+    <t># RF</t>
+  </si>
+  <si>
+    <t>RF1</t>
+  </si>
+  <si>
+    <t>RF3</t>
+  </si>
+  <si>
+    <t>RF4</t>
+  </si>
+  <si>
+    <t>RF5</t>
+  </si>
+  <si>
+    <t>RF6</t>
+  </si>
+  <si>
+    <t>RF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modificar de Estados de Los clientes</t>
+  </si>
+  <si>
+    <t>Descripción del requisto</t>
+  </si>
+  <si>
+    <t>Resultado del requisito</t>
+  </si>
+  <si>
+    <t>Afectacion de capa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se integra un apartado donde el cliente usuario determinará el estado del cliente: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario con rol de administrador deberá asignar un estado al cliente, este por defecto deberá ser integrado como activo, se deberá agregar un nuevo modulo </t>
+  </si>
+  <si>
+    <t>Todas</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>CAPAS</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Presentacion</t>
+  </si>
+  <si>
+    <t>Negocio</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>Entidades</t>
+  </si>
+  <si>
+    <t>Tablas Afec</t>
+  </si>
+  <si>
+    <t>datosrepresentantelegal</t>
+  </si>
+  <si>
+    <t>accionistas</t>
+  </si>
+  <si>
+    <t>beneficiariosfinales</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +390,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -324,11 +442,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -365,6 +494,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,11 +842,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3861A0-8375-4128-A93F-9BA9E76CA296}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
+  <dimension ref="A2:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -698,147 +1041,124 @@
     <col min="8" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G3" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="G5" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="G6" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -847,21 +1167,21 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G7" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -870,47 +1190,47 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="G9" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -919,193 +1239,222 @@
         <v>22</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G10" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="G11" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="G12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G19" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1113,4 +1462,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B757A7C-5DB0-4CAE-89BC-DF6FFAB8A725}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RF2- cambios en matriz de riesgos, accionistas y beneficiarios
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB7CFC8-3BE1-4C3A-B303-DC9121B60821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5A9D4-2098-44B8-9ED4-89E81518BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="116">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -134,9 +134,6 @@
     <t xml:space="preserve">Para calculo de matriz de riesgo se esta tomando N/A a BF, regla negocio aplicada,&lt;&lt;si no hay bf, se toma accionista&gt;&gt; </t>
   </si>
   <si>
-    <t xml:space="preserve">Aplicar regla de negocio, tomar la nacionalidad del del accionista mayoritarioExcp- si estos clientes tienen iguales acciones se debe de elegir de lo contrario agregar N/A </t>
-  </si>
-  <si>
     <t>Puede existir que el Cliente y RL Y AC sea FACTA mas de una vez</t>
   </si>
   <si>
@@ -381,13 +378,86 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Cerrada</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aplicar regla de negocio, tomar la nacionalidad del del accionista mayoritario 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>excepciones</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. si hay accionista mayoritarios con igual acciones (50/50) se deberá de tomar la nacionalidad del pais con mayor rango</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. los pic que no tienen bf, se debera de tomar el accionista mayoritario, aduntado excepcion 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3. si el cliente es ONG/entidad publica el registrador debera elegir la indicador y variables ambos para AC/BF.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +489,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,11 +650,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,7 +991,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,14 +1007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H1" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="H1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -951,25 +1036,25 @@
         <v>29</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="M2" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
@@ -992,25 +1077,25 @@
         <v>4</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1022,22 +1107,22 @@
       <c r="F4" s="26"/>
       <c r="G4" s="24"/>
       <c r="H4" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1049,22 +1134,22 @@
       <c r="F5" s="26"/>
       <c r="G5" s="24"/>
       <c r="H5" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1074,22 +1159,22 @@
       <c r="F6" s="26"/>
       <c r="G6" s="24"/>
       <c r="H6" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1099,22 +1184,22 @@
       <c r="F7" s="26"/>
       <c r="G7" s="24"/>
       <c r="H7" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1124,32 +1209,32 @@
       <c r="F8" s="26"/>
       <c r="G8" s="24"/>
       <c r="H8" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>114</v>
-      </c>
       <c r="K8" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A3:A8"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1161,7 +1246,7 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1281,7 @@
         <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1218,11 +1303,11 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="126.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1235,14 +1320,14 @@
       <c r="D4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>32</v>
+      <c r="E4" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1250,22 +1335,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -1288,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1311,7 +1396,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1334,7 +1419,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1357,7 +1442,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1380,7 +1465,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1397,13 +1482,13 @@
         <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1411,25 +1496,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="G12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1437,22 +1522,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="G13" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -1460,22 +1545,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="G14" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1483,22 +1568,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1506,22 +1591,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1529,22 +1614,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="D17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1552,22 +1637,22 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="F18" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1575,42 +1660,42 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="F19" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="G20" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1724,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -1648,84 +1733,84 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Desactivando el campo ID en actividad economica
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5A9D4-2098-44B8-9ED4-89E81518BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4671C530-46F0-4936-85BC-BD383FC1F612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
@@ -653,6 +653,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -667,18 +673,191 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1007,14 +1186,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1058,13 +1237,13 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1073,10 +1252,10 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="25" t="s">
         <v>109</v>
       </c>
       <c r="H3" s="16" t="s">
@@ -1099,13 +1278,13 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="19" t="s">
         <v>102</v>
       </c>
@@ -1126,13 +1305,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="19" t="s">
         <v>103</v>
       </c>
@@ -1153,11 +1332,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="24"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="19" t="s">
         <v>110</v>
       </c>
@@ -1178,11 +1357,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="19" t="s">
         <v>111</v>
       </c>
@@ -1203,11 +1382,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="24"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="19" t="s">
         <v>112</v>
       </c>
@@ -1245,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1529,7 @@
         <v>36</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -1373,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1699,6 +1878,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Abierta">
+      <formula>NOT(ISERROR(SEARCH("Abierta",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Cerrada">
+      <formula>NOT(ISERROR(SEARCH("Cerrada",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="En proceso">
+      <formula>NOT(ISERROR(SEARCH("En proceso",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
automatizacion del campo años negocio
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4671C530-46F0-4936-85BC-BD383FC1F612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BF1008-9825-40E3-95FE-04A5926E0DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -249,9 +249,6 @@
   </si>
   <si>
     <t>Integracion incompleta</t>
-  </si>
-  <si>
-    <t>50/100</t>
   </si>
   <si>
     <t>En proceso</t>
@@ -451,6 +448,12 @@
       </rPr>
       <t>3. si el cliente es ONG/entidad publica el registrador debera elegir la indicador y variables ambos para AC/BF.</t>
     </r>
+  </si>
+  <si>
+    <t>APROBADO</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -708,148 +711,6 @@
         <b/>
         <i val="0"/>
         <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
       </font>
       <fill>
         <patternFill>
@@ -1187,7 +1048,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H1" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
@@ -1218,22 +1079,22 @@
         <v>41</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="17" t="s">
-        <v>99</v>
-      </c>
       <c r="M2" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
@@ -1256,25 +1117,25 @@
         <v>4</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,22 +1147,22 @@
       <c r="F4" s="28"/>
       <c r="G4" s="26"/>
       <c r="H4" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1313,22 +1174,22 @@
       <c r="F5" s="28"/>
       <c r="G5" s="26"/>
       <c r="H5" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1338,22 +1199,22 @@
       <c r="F6" s="28"/>
       <c r="G6" s="26"/>
       <c r="H6" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1363,22 +1224,22 @@
       <c r="F7" s="28"/>
       <c r="G7" s="26"/>
       <c r="H7" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1388,22 +1249,22 @@
       <c r="F8" s="28"/>
       <c r="G8" s="26"/>
       <c r="H8" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>113</v>
-      </c>
       <c r="K8" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1424,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1298,8 @@
     <col min="5" max="5" width="51.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="17" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="6"/>
+    <col min="8" max="8" width="20.85546875" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1483,7 +1345,10 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="126.75" x14ac:dyDescent="0.25">
@@ -1500,13 +1365,13 @@
         <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1529,7 +1394,10 @@
         <v>36</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -1552,7 +1420,10 @@
         <v>10</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1575,7 +1446,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>42</v>
+        <v>113</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1690,10 +1564,10 @@
         <v>40</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1859,19 +1733,19 @@
     </row>
     <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>42</v>
@@ -1879,13 +1753,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Abierta">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Abierta">
       <formula>NOT(ISERROR(SEARCH("Abierta",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Cerrada">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Cerrada">
       <formula>NOT(ISERROR(SEARCH("Cerrada",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="En proceso">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="En proceso">
       <formula>NOT(ISERROR(SEARCH("En proceso",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1914,7 +1788,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -1923,13 +1797,13 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>41</v>
@@ -1937,70 +1811,70 @@
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementacion de RF1-estado cliente
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF8EDA-0A3C-40EC-91FF-D3D1714CC7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E953F44-B37F-4981-B7AC-12E19EE3A9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Modificacion pre-resolucion" sheetId="3" r:id="rId1"/>
+    <sheet name="Modificacion pre-resolucion" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="hallazgos" sheetId="1" r:id="rId2"/>
     <sheet name="RF" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Se debera de crear un apartado donde el cliente tendra que vizualizar el periodo de vencimiento de la cedula de identidad.</t>
+  </si>
+  <si>
+    <t>Si el cliente elige innactivo el estado del cliente no aparece/ para el cliente  solo se debe aplicar para activos e innactivos.</t>
   </si>
 </sst>
 </file>
@@ -692,6 +695,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,12 +721,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,14 +1092,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1140,13 +1143,13 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1155,10 +1158,10 @@
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="27" t="s">
         <v>102</v>
       </c>
       <c r="H3" s="16" t="s">
@@ -1181,13 +1184,13 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="26"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="19" t="s">
         <v>95</v>
       </c>
@@ -1208,13 +1211,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="26"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="19" t="s">
         <v>96</v>
       </c>
@@ -1235,11 +1238,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="26"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="19" t="s">
         <v>103</v>
       </c>
@@ -1260,11 +1263,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="26"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="19" t="s">
         <v>104</v>
       </c>
@@ -1285,11 +1288,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="26"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="19" t="s">
         <v>105</v>
       </c>
@@ -1327,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1812,23 +1815,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B757A7C-5DB0-4CAE-89BC-DF6FFAB8A725}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" style="29" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" style="22" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>73</v>
       </c>
@@ -1873,12 +1877,15 @@
       <c r="G2" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H2" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="22" t="s">
         <v>111</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1887,7 +1894,7 @@
       <c r="D3" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="23" t="s">
         <v>120</v>
       </c>
       <c r="F3" t="s">
@@ -1897,11 +1904,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="22" t="s">
         <v>115</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1910,7 +1917,7 @@
       <c r="D4" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="22" t="s">
         <v>122</v>
       </c>
       <c r="F4" t="s">
@@ -1920,83 +1927,83 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="22" t="s">
         <v>116</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="22" t="s">
         <v>117</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="22" t="s">
         <v>118</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="22" t="s">
         <v>119</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="22" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
quitar el componente de imprimir pantalla
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E953F44-B37F-4981-B7AC-12E19EE3A9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DC68FC-D291-4089-B48C-A66ECA266F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Modificacion pre-resolucion" sheetId="3" state="hidden" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="129">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -433,9 +433,6 @@
   </si>
   <si>
     <t>APROBADO</t>
-  </si>
-  <si>
-    <t>REVISAR</t>
   </si>
   <si>
     <t>Agregar de Campos adicionales a la BD, (Cotiza en Bolsa), Dignatarios/DIRECTORES/ Apoderados</t>
@@ -1330,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1491,7 @@
         <v>107</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1599,7 +1596,7 @@
       <c r="C12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -1625,7 +1622,7 @@
       <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -1648,7 +1645,7 @@
       <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -1658,7 +1655,10 @@
         <v>51</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>42</v>
+        <v>107</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
       <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="10" t="s">
@@ -1681,7 +1681,10 @@
         <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>42</v>
+        <v>107</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1694,7 +1697,7 @@
       <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -1717,7 +1720,7 @@
       <c r="C17" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1740,7 +1743,7 @@
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -1763,7 +1766,7 @@
       <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E19" s="10" t="s">
@@ -1777,22 +1780,22 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="10" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1817,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B757A7C-5DB0-4CAE-89BC-DF6FFAB8A725}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1837,7 +1840,7 @@
         <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -1878,24 +1881,24 @@
         <v>86</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" t="s">
         <v>85</v>
@@ -1909,16 +1912,16 @@
         <v>74</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>121</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>122</v>
       </c>
       <c r="F4" t="s">
         <v>85</v>
@@ -1932,16 +1935,16 @@
         <v>75</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>85</v>
@@ -1955,16 +1958,16 @@
         <v>76</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>126</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>85</v>
@@ -1978,7 +1981,7 @@
         <v>77</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
@@ -1989,16 +1992,16 @@
         <v>78</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>127</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>128</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
RF2- dignatarios, directores y apoderados -UI
</commit_message>
<xml_diff>
--- a/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
+++ b/RECURSOS/Hallazgos Pos-Despliegue/hallazgos_21-11-23.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sispla\RECURSOS\Hallazgos Pos-Despliegue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710E72A7-B06C-4CFB-8D5C-64B4F2D17716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB766F57-C21A-4848-9EF3-B46691841836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{2583B48C-DC56-4DE8-A3C6-531F45D33AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Modificacion pre-resolucion" sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="hallazgos" sheetId="1" r:id="rId2"/>
     <sheet name="RF" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="137">
   <si>
     <t>Implementación de matriz</t>
   </si>
@@ -206,9 +207,6 @@
     <t xml:space="preserve"> La impresión no se generá en una sola pagina, la impresión no contiene una vista estetica para impresión</t>
   </si>
   <si>
-    <t>Un usario que solo se le permite vista de DDC Puede realizar una impresión de DDC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error de codigo fuente </t>
   </si>
   <si>
@@ -267,9 +265,6 @@
   </si>
   <si>
     <t>RF5</t>
-  </si>
-  <si>
-    <t>RF6</t>
   </si>
   <si>
     <t>RF7</t>
@@ -456,9 +451,6 @@
     <t>Generar reportes de constancia de barridos mensuales (# cliente / hora de barrido / fecha)</t>
   </si>
   <si>
-    <t>Integrar a constancia indivuales, (RZ, Cliente_nat, RL, AC, BF, Empleados, Proveedores)</t>
-  </si>
-  <si>
     <t>Integrar la fecha proxima a vencerse de los Representante Legales</t>
   </si>
   <si>
@@ -490,13 +482,46 @@
   </si>
   <si>
     <t>Si el cliente elige innactivo el estado del cliente no aparece/ para el cliente  solo se debe aplicar para activos e innactivos.</t>
+  </si>
+  <si>
+    <t>Un usuario que solo se le permite vista de DDC Puede realizar una impresión de DDC</t>
+  </si>
+  <si>
+    <t>RF2: Agregar de Campos adicionales a la BD, (Cotiza en Bolsa), Dignatarios/DIRECTORES/ Apoderados</t>
+  </si>
+  <si>
+    <t>RF3: verificacion de en lista ofac/onu cliente_nat/rz/apoderado/rep/bf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF4: Generar constancia de barrido  individuales </t>
+  </si>
+  <si>
+    <t>RF5: Generar reportes de constancia de barridos mensuales (# cliente / hora de barrido / fecha)</t>
+  </si>
+  <si>
+    <t>RF6: Integrar a constancia indivuales, (RZ, Cliente_nat, RL, AC, BF, Empleados, Proveedores) completed 70%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF7: Integrar la fecha proxima a vencerse de los Representante Legales </t>
+  </si>
+  <si>
+    <t>Requisito</t>
+  </si>
+  <si>
+    <t>RF1: Modificar de Estados de Los clientes</t>
+  </si>
+  <si>
+    <t>No completado</t>
+  </si>
+  <si>
+    <t>Completado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +567,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -629,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -719,6 +752,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +766,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -756,7 +790,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1090,7 +1124,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H1" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1121,22 +1155,22 @@
         <v>41</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>92</v>
-      </c>
       <c r="M2" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
@@ -1159,25 +1193,25 @@
         <v>4</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,22 +1223,22 @@
       <c r="F4" s="30"/>
       <c r="G4" s="28"/>
       <c r="H4" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1216,22 +1250,22 @@
       <c r="F5" s="30"/>
       <c r="G5" s="28"/>
       <c r="H5" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1241,22 +1275,22 @@
       <c r="F6" s="30"/>
       <c r="G6" s="28"/>
       <c r="H6" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1266,22 +1300,22 @@
       <c r="F7" s="30"/>
       <c r="G7" s="28"/>
       <c r="H7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>106</v>
-      </c>
       <c r="K7" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1291,22 +1325,22 @@
       <c r="F8" s="30"/>
       <c r="G8" s="28"/>
       <c r="H8" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1327,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D94947-B970-4042-B4D8-E741B0D4E532}">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1401,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1387,10 +1421,10 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="126.75" x14ac:dyDescent="0.25">
@@ -1407,16 +1441,16 @@
         <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1436,13 +1470,13 @@
         <v>36</v>
       </c>
       <c r="G5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1462,13 +1496,13 @@
         <v>10</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1488,10 +1522,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1586,7 +1620,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1606,10 +1640,10 @@
         <v>40</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1635,7 +1669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="78.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1655,13 +1689,13 @@
         <v>51</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1675,16 +1709,16 @@
         <v>54</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1698,13 +1732,13 @@
         <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>42</v>
@@ -1715,16 +1749,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>47</v>
@@ -1738,19 +1772,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="F18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>42</v>
@@ -1761,19 +1795,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="F19" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>42</v>
@@ -1781,19 +1815,19 @@
     </row>
     <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>42</v>
@@ -1801,14 +1835,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Abierta">
-      <formula>NOT(ISERROR(SEARCH("Abierta",G1)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="En proceso">
+      <formula>NOT(ISERROR(SEARCH("En proceso",G1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Cerrada">
       <formula>NOT(ISERROR(SEARCH("Cerrada",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="En proceso">
-      <formula>NOT(ISERROR(SEARCH("En proceso",G1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Abierta">
+      <formula>NOT(ISERROR(SEARCH("Abierta",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1818,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B757A7C-5DB0-4CAE-89BC-DF6FFAB8A725}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,22 +1871,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>41</v>
@@ -1860,158 +1894,231 @@
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="H2" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>86</v>
+      <c r="D7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD22FBEE-1631-4064-BB9A-3A978B7013A4}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="99.140625" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>